<commit_message>
Encountered issue with running certain parsers
Varying the order of the term/type parsers seems to help. Using a parsing function in which a parser is passed works for some cases. Need to find the root of the issue.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-04july2016.xlsx
+++ b/time-labor/week-of-04july2016.xlsx
@@ -54,6 +54,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t xml:space="preserve">Weekly Time Record</t>
   </si>
@@ -151,10 +153,10 @@
     <t xml:space="preserve">Thursday</t>
   </si>
   <si>
-    <t xml:space="preserve">0800-1000,</t>
-  </si>
-  <si>
     <t xml:space="preserve">Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0800-1000, 1200-1300</t>
   </si>
   <si>
     <t xml:space="preserve">Saturday</t>
@@ -629,15 +631,15 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.1530612244898"/>
     <col collapsed="false" hidden="false" max="7" min="3" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.47959183673469"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -926,13 +928,17 @@
       <c r="B16" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="19" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="D16" s="20" t="n">
+        <v>0.625</v>
+      </c>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21" t="n">
         <f aca="false">IF((((D16-C16)+(F16-E16))*24)&gt;8,8,((D16-C16)+(F16-E16))*24)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H16" s="21" t="n">
         <f aca="false">IF(((D16-C16)+(F16-E16))*24&gt;8,((D16-C16)+(F16-E16))*24-8,0)</f>
@@ -942,20 +948,24 @@
       <c r="J16" s="23"/>
       <c r="K16" s="24"/>
       <c r="L16" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+        <v>28</v>
+      </c>
+      <c r="C17" s="19" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="D17" s="20" t="n">
+        <v>0.541666666666667</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21" t="n">
         <f aca="false">IF((((D17-C17)+(F17-E17))*24)&gt;8,8,((D17-C17)+(F17-E17))*24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H17" s="21" t="n">
         <f aca="false">IF(((D17-C17)+(F17-E17))*24&gt;8,((D17-C17)+(F17-E17))*24-8,0)</f>
@@ -964,19 +974,25 @@
       <c r="I17" s="22"/>
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
-      <c r="L17" s="0"/>
+      <c r="L17" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="20" t="n">
+        <v>0.583333333333333</v>
+      </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
       <c r="G18" s="21" t="n">
         <f aca="false">IF((((D18-C18)+(F18-E18))*24)&gt;8,8,((D18-C18)+(F18-E18))*24)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="21" t="n">
         <f aca="false">IF(((D18-C18)+(F18-E18))*24&gt;8,((D18-C18)+(F18-E18))*24-8,0)</f>
@@ -990,12 +1006,8 @@
       <c r="B19" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="20" t="n">
-        <v>0</v>
-      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21" t="n">
@@ -1020,7 +1032,7 @@
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1064,7 +1076,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1080,7 +1092,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>